<commit_message>
Para darlo a conocer por primera vez
</commit_message>
<xml_diff>
--- a/tablas.xlsx
+++ b/tablas.xlsx
@@ -8,12 +8,14 @@
   <sheets>
     <sheet name="firmas" r:id="rId3" sheetId="1"/>
     <sheet name="frec_ventas" r:id="rId4" sheetId="2"/>
+    <sheet name="contingencia_abs" r:id="rId5" sheetId="3"/>
+    <sheet name="contingencia_rel" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>FIRMA</t>
   </si>
@@ -121,6 +123,42 @@
   </si>
   <si>
     <t>[ 1823.36 , 1989.12 )</t>
+  </si>
+  <si>
+    <t>CIUDAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDIANA        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MICROEMPRESA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEQUEÑA        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAULE                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELOY ALFARO                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUAYAQUIL                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILAGRO                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NARANJITO                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMBORONDÓN                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SANTA LUCIA                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VELASCO IBARRA                                    </t>
   </si>
 </sst>
 </file>
@@ -623,4 +661,282 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>117.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>28.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="C4" t="n">
+        <v>72.67</v>
+      </c>
+      <c r="D4" t="n">
+        <v>17.39</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>